<commit_message>
updates excel save code
</commit_message>
<xml_diff>
--- a/Price Tracker/prices.xlsx
+++ b/Price Tracker/prices.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/66b97510e33847a9/Programming/Python/python-projects/Price Tracker/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="11_3AB5F0559F7C6C0E6C2948B64A51E6BC0D4E70BB" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C5715DD6-8FB8-412C-8D66-DCC2A304D8E0}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="11_3AB54DF5997A7ABEEC61D4144FD8FE7E100E77E9" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="2">
   <si>
     <t>Loveseat and Recliner</t>
   </si>
@@ -33,7 +33,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -66,7 +66,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -347,18 +347,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="95.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -368,11 +371,28 @@
       <c r="C1">
         <v>3599.97</v>
       </c>
-      <c r="E1">
+      <c r="D1">
         <v>3599.97</v>
       </c>
-      <c r="F1" s="1">
-        <v>45434.683638017967</v>
+      <c r="E1" s="1">
+        <v>45434.701642164349</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>3599.97</v>
+      </c>
+      <c r="D2">
+        <v>3599.97</v>
+      </c>
+      <c r="E2" s="1">
+        <v>45434.702188650903</v>
       </c>
     </row>
   </sheetData>

</xml_diff>